<commit_message>
fixed bug in M.save_excel preventing description or other columns from being saved
</commit_message>
<xml_diff>
--- a/Sub_Output - Copy.xlsx
+++ b/Sub_Output - Copy.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
   <si>
     <t>name</t>
   </si>
@@ -52,28 +52,49 @@
     <t>eps 4</t>
   </si>
   <si>
-    <t>test 1</t>
-  </si>
-  <si>
-    <t>test 2</t>
-  </si>
-  <si>
-    <t>test 3</t>
-  </si>
-  <si>
-    <t>test 4</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>m/s</t>
-  </si>
-  <si>
-    <t>sec</t>
-  </si>
-  <si>
-    <t>kg</t>
+    <t>W</t>
+  </si>
+  <si>
+    <t>current type</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>AC or DC</t>
+  </si>
+  <si>
+    <t>P min temp</t>
+  </si>
+  <si>
+    <t>P max temp</t>
+  </si>
+  <si>
+    <t>P max power</t>
+  </si>
+  <si>
+    <t>probe</t>
+  </si>
+  <si>
+    <t>O min temp</t>
+  </si>
+  <si>
+    <t>orbiter</t>
+  </si>
+  <si>
+    <t>O max temp</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>O max power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W </t>
+  </si>
+  <si>
+    <t>description</t>
   </si>
 </sst>
 </file>
@@ -107,7 +128,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -145,16 +166,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -583,66 +621,109 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>3.1428571428571428</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D8" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1006,7 +1087,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D5"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>